<commit_message>
fix: import product images
</commit_message>
<xml_diff>
--- a/public/templates/products_template.xlsx
+++ b/public/templates/products_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\ecommerce\storage\app\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\ecommerce\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACDBC4D-4DB4-4DFD-939A-4049D9F84003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA37901-48D5-4DA8-8F47-1FCC7964F918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>category_id</t>
+  </si>
+  <si>
+    <t>image_url</t>
   </si>
 </sst>
 </file>
@@ -357,15 +360,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,6 +386,9 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>